<commit_message>
Atualizaçao apenas de links
Atualizaçao apenas de links
</commit_message>
<xml_diff>
--- a/Entregavel_02/Sprint_03/PAP-PAR-PLANILHA_DE_AVALIACAO_GPR.xlsx
+++ b/Entregavel_02/Sprint_03/PAP-PAR-PLANILHA_DE_AVALIACAO_GPR.xlsx
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B992"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -5590,64 +5590,64 @@
     <hyperlink ref="B122" r:id="rId18"/>
     <hyperlink ref="B123" r:id="rId19"/>
     <hyperlink ref="B124" r:id="rId20"/>
-    <hyperlink ref="B120" r:id="rId21"/>
-    <hyperlink ref="B121" r:id="rId22"/>
-    <hyperlink ref="B135" r:id="rId23"/>
-    <hyperlink ref="B136" r:id="rId24"/>
-    <hyperlink ref="B130" r:id="rId25"/>
-    <hyperlink ref="B137" r:id="rId26"/>
-    <hyperlink ref="B138" r:id="rId27"/>
-    <hyperlink ref="B142" r:id="rId28"/>
-    <hyperlink ref="B143" r:id="rId29"/>
-    <hyperlink ref="B144" r:id="rId30"/>
-    <hyperlink ref="B154" r:id="rId31"/>
-    <hyperlink ref="B155" r:id="rId32"/>
-    <hyperlink ref="B175" r:id="rId33"/>
-    <hyperlink ref="B177" r:id="rId34"/>
-    <hyperlink ref="B186" r:id="rId35"/>
-    <hyperlink ref="B187" r:id="rId36"/>
-    <hyperlink ref="B188" r:id="rId37"/>
-    <hyperlink ref="B193" r:id="rId38"/>
-    <hyperlink ref="B215" r:id="rId39"/>
-    <hyperlink ref="A161:B161" r:id="rId40" display="Plano de Gerencia de Processo e Projeto"/>
-    <hyperlink ref="B199" r:id="rId41" display="Plano de Gerencia de Processo e Projeto"/>
-    <hyperlink ref="B207" r:id="rId42" display="Plano de Gerencia de Processo e Projeto"/>
-    <hyperlink ref="B210" r:id="rId43"/>
-    <hyperlink ref="B216" r:id="rId44"/>
-    <hyperlink ref="B58" r:id="rId45"/>
-    <hyperlink ref="B204" r:id="rId46"/>
-    <hyperlink ref="B231" r:id="rId47"/>
-    <hyperlink ref="B230" r:id="rId48"/>
-    <hyperlink ref="B226" r:id="rId49"/>
-    <hyperlink ref="B156" r:id="rId50"/>
-    <hyperlink ref="B169" r:id="rId51"/>
-    <hyperlink ref="B178" r:id="rId52"/>
-    <hyperlink ref="B185" r:id="rId53"/>
-    <hyperlink ref="B225" r:id="rId54"/>
-    <hyperlink ref="B13" r:id="rId55"/>
-    <hyperlink ref="B21" r:id="rId56"/>
-    <hyperlink ref="B28" r:id="rId57"/>
-    <hyperlink ref="B35" r:id="rId58"/>
-    <hyperlink ref="B42" r:id="rId59"/>
-    <hyperlink ref="B49" r:id="rId60"/>
-    <hyperlink ref="B56" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B70" r:id="rId63"/>
-    <hyperlink ref="B77" r:id="rId64"/>
-    <hyperlink ref="B85" r:id="rId65"/>
-    <hyperlink ref="B92" r:id="rId66"/>
-    <hyperlink ref="B128" r:id="rId67"/>
-    <hyperlink ref="B168" r:id="rId68"/>
-    <hyperlink ref="B179" r:id="rId69"/>
-    <hyperlink ref="B192" r:id="rId70"/>
-    <hyperlink ref="B202" r:id="rId71"/>
-    <hyperlink ref="B212" r:id="rId72"/>
-    <hyperlink ref="B222" r:id="rId73"/>
-    <hyperlink ref="B232" r:id="rId74"/>
-    <hyperlink ref="B238" r:id="rId75"/>
-    <hyperlink ref="B107" r:id="rId76"/>
-    <hyperlink ref="B176" r:id="rId77"/>
-    <hyperlink ref="B184" r:id="rId78"/>
+    <hyperlink ref="B121" r:id="rId21"/>
+    <hyperlink ref="B135" r:id="rId22"/>
+    <hyperlink ref="B136" r:id="rId23"/>
+    <hyperlink ref="B130" r:id="rId24"/>
+    <hyperlink ref="B137" r:id="rId25"/>
+    <hyperlink ref="B138" r:id="rId26"/>
+    <hyperlink ref="B142" r:id="rId27"/>
+    <hyperlink ref="B143" r:id="rId28"/>
+    <hyperlink ref="B144" r:id="rId29"/>
+    <hyperlink ref="B154" r:id="rId30"/>
+    <hyperlink ref="B155" r:id="rId31"/>
+    <hyperlink ref="B175" r:id="rId32"/>
+    <hyperlink ref="B177" r:id="rId33"/>
+    <hyperlink ref="B186" r:id="rId34"/>
+    <hyperlink ref="B187" r:id="rId35"/>
+    <hyperlink ref="B188" r:id="rId36"/>
+    <hyperlink ref="B193" r:id="rId37"/>
+    <hyperlink ref="B215" r:id="rId38"/>
+    <hyperlink ref="A161:B161" r:id="rId39" display="Plano de Gerencia de Processo e Projeto"/>
+    <hyperlink ref="B199" r:id="rId40" display="Plano de Gerencia de Processo e Projeto"/>
+    <hyperlink ref="B207" r:id="rId41" display="Plano de Gerencia de Processo e Projeto"/>
+    <hyperlink ref="B210" r:id="rId42"/>
+    <hyperlink ref="B216" r:id="rId43"/>
+    <hyperlink ref="B58" r:id="rId44"/>
+    <hyperlink ref="B204" r:id="rId45"/>
+    <hyperlink ref="B231" r:id="rId46"/>
+    <hyperlink ref="B230" r:id="rId47"/>
+    <hyperlink ref="B226" r:id="rId48"/>
+    <hyperlink ref="B13" r:id="rId49"/>
+    <hyperlink ref="B21" r:id="rId50"/>
+    <hyperlink ref="B28" r:id="rId51"/>
+    <hyperlink ref="B35" r:id="rId52"/>
+    <hyperlink ref="B42" r:id="rId53"/>
+    <hyperlink ref="B49" r:id="rId54"/>
+    <hyperlink ref="B56" r:id="rId55"/>
+    <hyperlink ref="B63" r:id="rId56"/>
+    <hyperlink ref="B70" r:id="rId57"/>
+    <hyperlink ref="B77" r:id="rId58"/>
+    <hyperlink ref="B85" r:id="rId59"/>
+    <hyperlink ref="B92" r:id="rId60"/>
+    <hyperlink ref="B128" r:id="rId61"/>
+    <hyperlink ref="B168" r:id="rId62"/>
+    <hyperlink ref="B179" r:id="rId63"/>
+    <hyperlink ref="B192" r:id="rId64"/>
+    <hyperlink ref="B202" r:id="rId65"/>
+    <hyperlink ref="B212" r:id="rId66"/>
+    <hyperlink ref="B222" r:id="rId67"/>
+    <hyperlink ref="B232" r:id="rId68"/>
+    <hyperlink ref="B238" r:id="rId69"/>
+    <hyperlink ref="B107" r:id="rId70"/>
+    <hyperlink ref="B176" r:id="rId71"/>
+    <hyperlink ref="B184" r:id="rId72"/>
+    <hyperlink ref="B120" r:id="rId73"/>
+    <hyperlink ref="B156" r:id="rId74"/>
+    <hyperlink ref="B169" r:id="rId75"/>
+    <hyperlink ref="B178" r:id="rId76"/>
+    <hyperlink ref="B185" r:id="rId77"/>
+    <hyperlink ref="B225" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId79"/>

</xml_diff>